<commit_message>
Added current and voltage calculations for double conjugate-T antenna (resonant double loop). Results correctly checked vs Designer. (Excel Table updated).
</commit_message>
<xml_diff>
--- a/icrh/data/TOPICA/ToreSupra_WEST/WEST_ICRH_Compilation_resultats_designer.xlsx
+++ b/icrh/data/TOPICA/ToreSupra_WEST/WEST_ICRH_Compilation_resultats_designer.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="25875" windowHeight="10290"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="25872" windowHeight="10296" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="22116" windowHeight="9528" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Designer data" sheetId="1" r:id="rId1"/>
+    <sheet name="Python model" sheetId="2" r:id="rId2"/>
+    <sheet name="Capacitor Current vs Rc" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$A$1:$AS$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Designer data'!$A$1:$AS$40</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="68">
   <si>
     <t>Frequency [MHz]</t>
   </si>
@@ -215,6 +216,15 @@
   <si>
     <t>Zs_TSproto12_55MHz_LAD9-5cm.txt</t>
   </si>
+  <si>
+    <t>V2B [kV]</t>
+  </si>
+  <si>
+    <t>Active S1 Mag [dB]</t>
+  </si>
+  <si>
+    <t>Active S2 Mag [dB]</t>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +386,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +427,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -449,7 +483,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>(data!$D$2:$D$9,data!$D$20:$D$25)</c:f>
+              <c:f>('Designer data'!$D$2:$D$9,'Designer data'!$D$20:$D$25)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -500,7 +534,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(data!$AS$2:$AS$9,data!$AS$20:$AS$25)</c:f>
+              <c:f>('Designer data'!$AS$2:$AS$9,'Designer data'!$AS$20:$AS$25)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -564,7 +598,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>(data!$D$11:$D$18,data!$D$30:$D$35)</c:f>
+              <c:f>('Designer data'!$D$11:$D$18,'Designer data'!$D$30:$D$35)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
@@ -615,7 +649,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(data!$AS$11:$AS$18,data!$AS$30:$AS$35)</c:f>
+              <c:f>('Designer data'!$AS$11:$AS$18,'Designer data'!$AS$30:$AS$35)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -674,11 +708,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121625216"/>
-        <c:axId val="121623680"/>
+        <c:axId val="163863936"/>
+        <c:axId val="163898496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121625216"/>
+        <c:axId val="163863936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,12 +722,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121623680"/>
+        <c:crossAx val="163898496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121623680"/>
+        <c:axId val="163898496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,7 +738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121625216"/>
+        <c:crossAx val="163863936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -724,6 +758,1069 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Max Power for 1/2 antenna</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3551416429368955E-2"/>
+          <c:y val="1.3888888888888888E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>real match</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Designer data'!$D$2:$D$9,'Designer data'!$D$20:$D$25)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.394233691326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.80477500408199998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7076141356200001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42156602891900002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.87657298072099998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.81570768537</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Designer data'!$AS$2:$AS$9,'Designer data'!$AS$20:$AS$25)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>imag match</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Designer data'!$D$11:$D$18,'Designer data'!$D$30:$D$35)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.394233691326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.80477500408199998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7076141356200001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42156602891900002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.87657298072099998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.81570768537</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Designer data'!$AS$11:$AS$18,'Designer data'!$AS$30:$AS$35)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="40947072"/>
+        <c:axId val="41751680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="40947072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41751680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="41751680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40947072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Designer IC1B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Designer data'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Designer data'!$X$2:$X$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0552448627574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90977543251404303</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81402504110458296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74806293595040596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69176690321586798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61431139198052898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63293335067704304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68025976783866204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Designer IC1H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Designer data'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Designer data'!$Y$2:$Y$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2756133198398001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.19155255695542</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1408805444374801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0914272759300601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05062866160053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0088970774060999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94933871859201502</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86839570102111896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Designer IC2B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Designer data'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Designer data'!$Z$2:$Z$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3672617491218699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.26710404708211</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1863255341013399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1192738158967299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.11420351506337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.06991561580172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.04829110690222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.03060295780532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Designer IC2H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Designer data'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Designer data'!$AA$2:$AA$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.12658105865777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99222318392600495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93332341247747097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89399848653264202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80299527499373702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72866749637679196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70060021419529706</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64154305718384197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Python IC1H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Python model'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Python model'!$T$2:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.16585518705835</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0261165882519701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1826526981068799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97135899803911196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1212418709902401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0745872560959699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0603673743791</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86491585875233101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Python IC1B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Python model'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Python model'!$U$2:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.10390590779383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96325862604463097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0645420592016199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1700413341404601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.958924118713817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86700511757217202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84319488535345499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84768438692215697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Python IC2H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Python model'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Python model'!$V$2:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3434397395942399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2206442259115899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94457560944360797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2238644545366399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86099889594613499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78471759517059403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77326033255209403</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.50821917360503799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Python IC2B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Python model'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0625752451781001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3351907809458401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.56728058309068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.81219298226804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0529370827241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4462693228308301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6533946851368002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.90565590947116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Python model'!$W$2:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.29031211126889</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.16435727283803</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2741566849569299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92769022158547199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.19762861920816</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.13385388003528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1013538463852</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49171676519700003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="94311936"/>
+        <c:axId val="154650112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="94311936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154650112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="154650112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94311936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="42" workbookViewId="1" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -761,8 +1858,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>294409</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>178376</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>64076</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1053,29 +2214,34 @@
   </sheetPr>
   <dimension ref="A1:AS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X54" sqref="X54"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18:XFD18"/>
+    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="23.42578125" style="23" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="20.21875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="1"/>
-    <col min="10" max="11" width="9.140625" style="6"/>
-    <col min="12" max="15" width="9.140625" style="14"/>
-    <col min="16" max="23" width="9.140625" style="1"/>
-    <col min="24" max="35" width="9.140625" style="11"/>
-    <col min="36" max="36" width="12.140625" style="1" customWidth="1"/>
-    <col min="37" max="40" width="9.140625" style="8"/>
-    <col min="41" max="44" width="9.140625" style="9"/>
-    <col min="45" max="45" width="9.140625" style="12"/>
-    <col min="46" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="9" width="9.109375" style="1"/>
+    <col min="10" max="11" width="9.109375" style="6"/>
+    <col min="12" max="15" width="9.109375" style="14"/>
+    <col min="16" max="23" width="9.109375" style="1"/>
+    <col min="24" max="27" width="9.109375" style="11"/>
+    <col min="28" max="35" width="9.109375" style="12"/>
+    <col min="36" max="36" width="12.109375" style="1" customWidth="1"/>
+    <col min="37" max="40" width="9.109375" style="8"/>
+    <col min="41" max="44" width="9.109375" style="9"/>
+    <col min="45" max="45" width="9.109375" style="12"/>
+    <col min="46" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1160,28 +2326,28 @@
       <c r="AA1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AC1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AD1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AE1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AF1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AG1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AH1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AI1" s="28" t="s">
         <v>26</v>
       </c>
       <c r="AJ1" s="3" t="s">
@@ -1215,7 +2381,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1299,22 +2465,22 @@
       <c r="AA2" s="11">
         <v>1.12658105865777</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AD2" s="12">
         <v>0.94264879392524104</v>
       </c>
-      <c r="AE2" s="11">
+      <c r="AE2" s="12">
         <v>993178.77976856299</v>
       </c>
-      <c r="AF2" s="11">
+      <c r="AF2" s="12">
         <v>0.296363855451103</v>
       </c>
-      <c r="AG2" s="11">
+      <c r="AG2" s="12">
         <v>0.30283942608378001</v>
       </c>
-      <c r="AH2" s="11">
+      <c r="AH2" s="12">
         <v>0.29621148155794402</v>
       </c>
-      <c r="AI2" s="11">
+      <c r="AI2" s="12">
         <v>0.30291676613284202</v>
       </c>
       <c r="AJ2" s="1">
@@ -1349,7 +2515,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1433,28 +2599,28 @@
       <c r="AA3" s="11">
         <v>0.99222318392600495</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="12">
         <v>0.17</v>
       </c>
-      <c r="AC3" s="11">
+      <c r="AC3" s="12">
         <v>0.17</v>
       </c>
-      <c r="AD3" s="11">
+      <c r="AD3" s="12">
         <v>1.0047862991754899</v>
       </c>
-      <c r="AE3" s="11">
+      <c r="AE3" s="12">
         <v>1.03900498494649</v>
       </c>
-      <c r="AF3" s="11">
+      <c r="AF3" s="12">
         <v>0.29370908785486499</v>
       </c>
-      <c r="AG3" s="11">
+      <c r="AG3" s="12">
         <v>0.29478948785616499</v>
       </c>
-      <c r="AH3" s="11">
+      <c r="AH3" s="12">
         <v>0.293938242210739</v>
       </c>
-      <c r="AI3" s="11">
+      <c r="AI3" s="12">
         <v>0.29520876720592998</v>
       </c>
       <c r="AJ3" s="1">
@@ -1489,7 +2655,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1573,28 +2739,28 @@
       <c r="AA4" s="11">
         <v>0.93332341247747097</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="12">
         <v>0.17673404519508201</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="12">
         <v>0.182588263202039</v>
       </c>
-      <c r="AD4" s="11">
+      <c r="AD4" s="12">
         <v>1.0504675385159501</v>
       </c>
-      <c r="AE4" s="11">
+      <c r="AE4" s="12">
         <v>1.0652184249580401</v>
       </c>
-      <c r="AF4" s="11">
+      <c r="AF4" s="12">
         <v>0.28996059654852901</v>
       </c>
-      <c r="AG4" s="11">
+      <c r="AG4" s="12">
         <v>0.280617548600957</v>
       </c>
-      <c r="AH4" s="11">
+      <c r="AH4" s="12">
         <v>0.29049554712957498</v>
       </c>
-      <c r="AI4" s="11">
+      <c r="AI4" s="12">
         <v>0.28133585468637501</v>
       </c>
       <c r="AK4" s="8">
@@ -1626,7 +2792,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -1710,28 +2876,28 @@
       <c r="AA5" s="11">
         <v>0.89399848653264202</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AB5" s="12">
         <v>0.18194274803846799</v>
       </c>
-      <c r="AC5" s="11">
+      <c r="AC5" s="12">
         <v>0.18891538390885701</v>
       </c>
-      <c r="AD5" s="11">
+      <c r="AD5" s="12">
         <v>1.0806487266149001</v>
       </c>
-      <c r="AE5" s="11">
+      <c r="AE5" s="12">
         <v>1.07321038761795</v>
       </c>
-      <c r="AF5" s="11">
+      <c r="AF5" s="12">
         <v>0.28370360159779401</v>
       </c>
-      <c r="AG5" s="11">
+      <c r="AG5" s="12">
         <v>0.270793369300244</v>
       </c>
-      <c r="AH5" s="11">
+      <c r="AH5" s="12">
         <v>0.28448108608534101</v>
       </c>
-      <c r="AI5" s="11">
+      <c r="AI5" s="12">
         <v>0.27165873412129199</v>
       </c>
       <c r="AK5" s="8">
@@ -1763,7 +2929,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -1847,28 +3013,28 @@
       <c r="AA6" s="11">
         <v>0.80299527499373702</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="12">
         <v>0.18644782348856601</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="12">
         <v>0.190367704428725</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6" s="12">
         <v>1.1039061850454699</v>
       </c>
-      <c r="AE6" s="11">
+      <c r="AE6" s="12">
         <v>1.10724767925602</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6" s="12">
         <v>0.27830055290097599</v>
       </c>
-      <c r="AG6" s="11">
+      <c r="AG6" s="12">
         <v>0.27199619812998699</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AH6" s="12">
         <v>0.279278378101466</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6" s="12">
         <v>0.27306315101591899</v>
       </c>
       <c r="AK6" s="8" t="s">
@@ -1900,7 +3066,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -1984,28 +3150,28 @@
       <c r="AA7" s="11">
         <v>0.72866749637679196</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="12">
         <v>0.19166398804821899</v>
       </c>
-      <c r="AC7" s="11">
+      <c r="AC7" s="12">
         <v>0.195811932773133</v>
       </c>
-      <c r="AD7" s="11">
+      <c r="AD7" s="12">
         <v>1.1319479246237401</v>
       </c>
-      <c r="AE7" s="11">
+      <c r="AE7" s="12">
         <v>1.12560423102951</v>
       </c>
-      <c r="AF7" s="11">
+      <c r="AF7" s="12">
         <v>0.27295660537358202</v>
       </c>
-      <c r="AG7" s="11">
+      <c r="AG7" s="12">
         <v>0.26514120005001701</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AH7" s="12">
         <v>0.27416891276165001</v>
       </c>
-      <c r="AI7" s="11">
+      <c r="AI7" s="12">
         <v>0.26640087397607598</v>
       </c>
       <c r="AK7" s="8" t="s">
@@ -2037,7 +3203,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
@@ -2121,28 +3287,28 @@
       <c r="AA8" s="11">
         <v>0.70060021419529706</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="12">
         <v>0.199807257926781</v>
       </c>
-      <c r="AC8" s="11">
+      <c r="AC8" s="12">
         <v>0.19951883732445599</v>
       </c>
-      <c r="AD8" s="11">
+      <c r="AD8" s="12">
         <v>1.1107776264153499</v>
       </c>
-      <c r="AE8" s="11">
+      <c r="AE8" s="12">
         <v>1.1137172738076999</v>
       </c>
-      <c r="AF8" s="11">
+      <c r="AF8" s="12">
         <v>0.25637831933567501</v>
       </c>
-      <c r="AG8" s="11">
+      <c r="AG8" s="12">
         <v>0.257263944883377</v>
       </c>
-      <c r="AH8" s="11">
+      <c r="AH8" s="12">
         <v>0.25763953503468501</v>
       </c>
-      <c r="AI8" s="11">
+      <c r="AI8" s="12">
         <v>0.258534590223859</v>
       </c>
       <c r="AK8" s="8" t="s">
@@ -2174,7 +3340,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -2258,28 +3424,28 @@
       <c r="AA9" s="11">
         <v>0.64154305718384197</v>
       </c>
-      <c r="AB9" s="11">
+      <c r="AB9" s="12">
         <v>0.208624112371289</v>
       </c>
-      <c r="AC9" s="11">
+      <c r="AC9" s="12">
         <v>0.20616359475382401</v>
       </c>
-      <c r="AD9" s="11">
+      <c r="AD9" s="12">
         <v>1.09863168549006</v>
       </c>
-      <c r="AE9" s="11">
+      <c r="AE9" s="12">
         <v>1.12333808676361</v>
       </c>
-      <c r="AF9" s="11">
+      <c r="AF9" s="12">
         <v>0.239644480499458</v>
       </c>
-      <c r="AG9" s="11">
+      <c r="AG9" s="12">
         <v>0.24738463599588101</v>
       </c>
-      <c r="AH9" s="11">
+      <c r="AH9" s="12">
         <v>0.24101016195969099</v>
       </c>
-      <c r="AI9" s="11">
+      <c r="AI9" s="12">
         <v>0.24883081588960801</v>
       </c>
       <c r="AJ9" s="1">
@@ -2314,18 +3480,26 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="10" spans="1:45" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="D10" s="21"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
       <c r="AO10" s="9"/>
       <c r="AP10" s="9"/>
       <c r="AQ10" s="9"/>
       <c r="AR10" s="9"/>
       <c r="AS10" s="12"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -2409,22 +3583,22 @@
       <c r="AA11" s="11">
         <v>1.2082078497600099</v>
       </c>
-      <c r="AD11" s="11">
+      <c r="AD11" s="12">
         <v>0.72611856285154797</v>
       </c>
-      <c r="AE11" s="11">
+      <c r="AE11" s="12">
         <v>779685.52239634399</v>
       </c>
-      <c r="AF11" s="11">
+      <c r="AF11" s="12">
         <v>0.293065366219812</v>
       </c>
-      <c r="AG11" s="11">
+      <c r="AG11" s="12">
         <v>0.29483662892969498</v>
       </c>
-      <c r="AH11" s="11">
+      <c r="AH11" s="12">
         <v>0.29175769436952298</v>
       </c>
-      <c r="AI11" s="11">
+      <c r="AI11" s="12">
         <v>0.29379934153165399</v>
       </c>
       <c r="AJ11" s="1">
@@ -2459,7 +3633,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -2543,28 +3717,28 @@
       <c r="AA12" s="11">
         <v>1.09566103743809</v>
       </c>
-      <c r="AB12" s="11">
+      <c r="AB12" s="12">
         <v>0.17900148205029701</v>
       </c>
-      <c r="AC12" s="11">
+      <c r="AC12" s="12">
         <v>0.17930844456822601</v>
       </c>
-      <c r="AD12" s="11">
+      <c r="AD12" s="12">
         <v>0.80010576876367501</v>
       </c>
-      <c r="AE12" s="11">
+      <c r="AE12" s="12">
         <v>828150.96804169298</v>
       </c>
-      <c r="AF12" s="11">
+      <c r="AF12" s="12">
         <v>0.29335548835201902</v>
       </c>
-      <c r="AG12" s="11">
+      <c r="AG12" s="12">
         <v>0.28873736052286803</v>
       </c>
-      <c r="AH12" s="11">
+      <c r="AH12" s="12">
         <v>0.29243684742278397</v>
       </c>
-      <c r="AI12" s="11">
+      <c r="AI12" s="12">
         <v>0.28800239346970402</v>
       </c>
       <c r="AJ12" s="1">
@@ -2599,7 +3773,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -2683,28 +3857,28 @@
       <c r="AA13" s="11">
         <v>1.02678547225675</v>
       </c>
-      <c r="AB13" s="11">
+      <c r="AB13" s="12">
         <v>0.17792992618721501</v>
       </c>
-      <c r="AC13" s="11">
+      <c r="AC13" s="12">
         <v>0.18037567146969299</v>
       </c>
-      <c r="AD13" s="11">
+      <c r="AD13" s="12">
         <v>0.84950185495013497</v>
       </c>
-      <c r="AE13" s="11">
+      <c r="AE13" s="12">
         <v>870525.59082993504</v>
       </c>
-      <c r="AF13" s="11">
+      <c r="AF13" s="12">
         <v>0.28961893634971098</v>
       </c>
-      <c r="AG13" s="11">
+      <c r="AG13" s="12">
         <v>0.28233253064103098</v>
       </c>
-      <c r="AH13" s="11">
+      <c r="AH13" s="12">
         <v>0.28899603758079601</v>
       </c>
-      <c r="AI13" s="11">
+      <c r="AI13" s="12">
         <v>0.28188069337428201</v>
       </c>
       <c r="AK13" s="8">
@@ -2736,7 +3910,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2820,28 +3994,28 @@
       <c r="AA14" s="11">
         <v>0.97966159741888703</v>
       </c>
-      <c r="AB14" s="11">
+      <c r="AB14" s="12">
         <v>0.177588729543389</v>
       </c>
-      <c r="AC14" s="11">
+      <c r="AC14" s="12">
         <v>0.18433292854739</v>
       </c>
-      <c r="AD14" s="11">
+      <c r="AD14" s="12">
         <v>0.89883799862941105</v>
       </c>
-      <c r="AE14" s="11">
+      <c r="AE14" s="12">
         <v>905495.976588786</v>
       </c>
-      <c r="AF14" s="11">
+      <c r="AF14" s="12">
         <v>0.287486383187882</v>
       </c>
-      <c r="AG14" s="11">
+      <c r="AG14" s="12">
         <v>0.27303591655708997</v>
       </c>
-      <c r="AH14" s="11">
+      <c r="AH14" s="12">
         <v>0.28715358207972602</v>
       </c>
-      <c r="AI14" s="11">
+      <c r="AI14" s="12">
         <v>0.27285338870422099</v>
       </c>
       <c r="AK14" s="8">
@@ -2873,7 +4047,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -2957,28 +4131,28 @@
       <c r="AA15" s="11">
         <v>0.898630580461654</v>
       </c>
-      <c r="AB15" s="11">
+      <c r="AB15" s="12">
         <v>0.17201098288254699</v>
       </c>
-      <c r="AC15" s="11">
+      <c r="AC15" s="12">
         <v>0.179476456169891</v>
       </c>
-      <c r="AD15" s="11">
+      <c r="AD15" s="12">
         <v>0.90857338858811099</v>
       </c>
-      <c r="AE15" s="11">
+      <c r="AE15" s="12">
         <v>906580.31887952203</v>
       </c>
-      <c r="AF15" s="11">
+      <c r="AF15" s="12">
         <v>0.27495472970908602</v>
       </c>
-      <c r="AG15" s="11">
+      <c r="AG15" s="12">
         <v>0.26002418716490899</v>
       </c>
-      <c r="AH15" s="11">
+      <c r="AH15" s="12">
         <v>0.27489039296693002</v>
       </c>
-      <c r="AI15" s="11">
+      <c r="AI15" s="12">
         <v>0.260071332077287</v>
       </c>
       <c r="AK15" s="8">
@@ -3010,7 +4184,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -3094,28 +4268,28 @@
       <c r="AA16" s="11">
         <v>0.84933377703897295</v>
       </c>
-      <c r="AB16" s="11">
+      <c r="AB16" s="12">
         <v>0.17171001965639199</v>
       </c>
-      <c r="AC16" s="11">
+      <c r="AC16" s="12">
         <v>0.18276623271914</v>
       </c>
-      <c r="AD16" s="11">
+      <c r="AD16" s="12">
         <v>0.96052429472841605</v>
       </c>
-      <c r="AE16" s="11">
+      <c r="AE16" s="12">
         <v>932987.99741963495</v>
       </c>
-      <c r="AF16" s="11">
+      <c r="AF16" s="12">
         <v>0.275944372909534</v>
       </c>
-      <c r="AG16" s="11">
+      <c r="AG16" s="12">
         <v>0.254025517638228</v>
       </c>
-      <c r="AH16" s="11">
+      <c r="AH16" s="12">
         <v>0.27617712823917001</v>
       </c>
-      <c r="AI16" s="11">
+      <c r="AI16" s="12">
         <v>0.25428541613962702</v>
       </c>
       <c r="AK16" s="8">
@@ -3147,7 +4321,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -3231,28 +4405,28 @@
       <c r="AA17" s="11">
         <v>0.85599466956091497</v>
       </c>
-      <c r="AB17" s="11">
+      <c r="AB17" s="12">
         <v>0.179937268914209</v>
       </c>
-      <c r="AC17" s="11">
+      <c r="AC17" s="12">
         <v>0.189439590962201</v>
       </c>
-      <c r="AD17" s="11">
+      <c r="AD17" s="12">
         <v>0.96703865170774495</v>
       </c>
-      <c r="AE17" s="11">
+      <c r="AE17" s="12">
         <v>928287.64860233804</v>
       </c>
-      <c r="AF17" s="11">
+      <c r="AF17" s="12">
         <v>0.26068816893714503</v>
       </c>
-      <c r="AG17" s="11">
+      <c r="AG17" s="12">
         <v>0.241119501599633</v>
       </c>
-      <c r="AH17" s="11">
+      <c r="AH17" s="12">
         <v>0.26110039518811901</v>
       </c>
-      <c r="AI17" s="11">
+      <c r="AI17" s="12">
         <v>0.24145878709960999</v>
       </c>
       <c r="AK17" s="8">
@@ -3284,7 +4458,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -3368,28 +4542,28 @@
       <c r="AA18" s="11">
         <v>0.82622612354894998</v>
       </c>
-      <c r="AB18" s="11">
+      <c r="AB18" s="12">
         <v>0.18763313832026901</v>
       </c>
-      <c r="AC18" s="11">
+      <c r="AC18" s="12">
         <v>0.192581599661618</v>
       </c>
-      <c r="AD18" s="11">
+      <c r="AD18" s="12">
         <v>0.97212861490945701</v>
       </c>
-      <c r="AE18" s="11">
+      <c r="AE18" s="12">
         <v>944661.21282667201</v>
       </c>
-      <c r="AF18" s="11">
+      <c r="AF18" s="12">
         <v>0.24671810731607999</v>
       </c>
-      <c r="AG18" s="11">
+      <c r="AG18" s="12">
         <v>0.23590702402477701</v>
       </c>
-      <c r="AH18" s="11">
+      <c r="AH18" s="12">
         <v>0.247291376910697</v>
       </c>
-      <c r="AI18" s="11">
+      <c r="AI18" s="12">
         <v>0.23639792135257601</v>
       </c>
       <c r="AK18" s="8">
@@ -3421,11 +4595,19 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="19" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="D19" s="22"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>59</v>
       </c>
@@ -3509,28 +4691,28 @@
       <c r="AA20" s="11">
         <v>2.0061224789808101</v>
       </c>
-      <c r="AB20" s="11">
+      <c r="AB20" s="12">
         <v>0.28154611409783198</v>
       </c>
-      <c r="AC20" s="11">
+      <c r="AC20" s="12">
         <v>0.27368895788999298</v>
       </c>
-      <c r="AD20" s="11">
+      <c r="AD20" s="12">
         <v>0.94593879397510205</v>
       </c>
-      <c r="AE20" s="11">
+      <c r="AE20" s="12">
         <v>864548.25541526999</v>
       </c>
-      <c r="AF20" s="11">
+      <c r="AF20" s="12">
         <v>0.112533622905714</v>
       </c>
-      <c r="AG20" s="11">
+      <c r="AG20" s="12">
         <v>0.127854645870385</v>
       </c>
-      <c r="AH20" s="11">
+      <c r="AH20" s="12">
         <v>0.11320284371108701</v>
       </c>
-      <c r="AI20" s="11">
+      <c r="AI20" s="12">
         <v>0.12751370105113399</v>
       </c>
       <c r="AK20" s="8">
@@ -3562,7 +4744,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>60</v>
       </c>
@@ -3646,28 +4828,28 @@
       <c r="AA21" s="11">
         <v>1.5679830992263999</v>
       </c>
-      <c r="AB21" s="11">
+      <c r="AB21" s="12">
         <v>0.24188611012370601</v>
       </c>
-      <c r="AC21" s="11">
+      <c r="AC21" s="12">
         <v>0.234547142555914</v>
       </c>
-      <c r="AD21" s="11">
+      <c r="AD21" s="12">
         <v>0.83448778651158695</v>
       </c>
-      <c r="AE21" s="11">
+      <c r="AE21" s="12">
         <v>848785.82876791002</v>
       </c>
-      <c r="AF21" s="11">
+      <c r="AF21" s="12">
         <v>0.19217002645758</v>
       </c>
-      <c r="AG21" s="11">
+      <c r="AG21" s="12">
         <v>0.20635605848667801</v>
       </c>
-      <c r="AH21" s="11">
+      <c r="AH21" s="12">
         <v>0.19166255547541999</v>
       </c>
-      <c r="AI21" s="11">
+      <c r="AI21" s="12">
         <v>0.20593467253933501</v>
       </c>
       <c r="AK21" s="8">
@@ -3699,7 +4881,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>61</v>
       </c>
@@ -3783,28 +4965,28 @@
       <c r="AA22" s="11">
         <v>1.0852117287734899</v>
       </c>
-      <c r="AB22" s="11">
+      <c r="AB22" s="12">
         <v>0.22008734289192</v>
       </c>
-      <c r="AC22" s="11">
+      <c r="AC22" s="12">
         <v>0.21742074776961701</v>
       </c>
-      <c r="AD22" s="11">
+      <c r="AD22" s="12">
         <v>1.0050791821488101</v>
       </c>
-      <c r="AE22" s="11">
+      <c r="AE22" s="12">
         <v>1.0112926037004599</v>
       </c>
-      <c r="AF22" s="11">
+      <c r="AF22" s="12">
         <v>0.23563175984707699</v>
       </c>
-      <c r="AG22" s="11">
+      <c r="AG22" s="12">
         <v>0.24100346323566399</v>
       </c>
-      <c r="AH22" s="11">
+      <c r="AH22" s="12">
         <v>0.236186534504255</v>
       </c>
-      <c r="AI22" s="11">
+      <c r="AI22" s="12">
         <v>0.24155790144408401</v>
       </c>
       <c r="AK22" s="8">
@@ -3836,7 +5018,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>62</v>
       </c>
@@ -3920,28 +5102,28 @@
       <c r="AA23" s="11">
         <v>1.96368600761442</v>
       </c>
-      <c r="AB23" s="11">
+      <c r="AB23" s="12">
         <v>0.280145569781378</v>
       </c>
-      <c r="AC23" s="11">
+      <c r="AC23" s="12">
         <v>0.27120794084914801</v>
       </c>
-      <c r="AD23" s="11">
+      <c r="AD23" s="12">
         <v>0.92356476558895095</v>
       </c>
-      <c r="AE23" s="11">
+      <c r="AE23" s="12">
         <v>851708.79430755298</v>
       </c>
-      <c r="AF23" s="11">
+      <c r="AF23" s="12">
         <v>0.11481084030472</v>
       </c>
-      <c r="AG23" s="11">
+      <c r="AG23" s="12">
         <v>0.133407873962401</v>
       </c>
-      <c r="AH23" s="11">
+      <c r="AH23" s="12">
         <v>0.115173726556397</v>
       </c>
-      <c r="AI23" s="11">
+      <c r="AI23" s="12">
         <v>0.13294323300201499</v>
       </c>
       <c r="AK23" s="8">
@@ -3973,7 +5155,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>63</v>
       </c>
@@ -4057,28 +5239,28 @@
       <c r="AA24" s="11">
         <v>1.5011717143726599</v>
       </c>
-      <c r="AB24" s="11">
+      <c r="AB24" s="12">
         <v>0.23510616339374901</v>
       </c>
-      <c r="AC24" s="11">
+      <c r="AC24" s="12">
         <v>0.22938610324898301</v>
       </c>
-      <c r="AD24" s="11">
+      <c r="AD24" s="12">
         <v>0.82665614287744205</v>
       </c>
-      <c r="AE24" s="11">
+      <c r="AE24" s="12">
         <v>853576.40747582295</v>
       </c>
-      <c r="AF24" s="11">
+      <c r="AF24" s="12">
         <v>0.206599308324423</v>
       </c>
-      <c r="AG24" s="11">
+      <c r="AG24" s="12">
         <v>0.216865826461489</v>
       </c>
-      <c r="AH24" s="11">
+      <c r="AH24" s="12">
         <v>0.20600798252667399</v>
       </c>
-      <c r="AI24" s="11">
+      <c r="AI24" s="12">
         <v>0.216446674587745</v>
       </c>
       <c r="AK24" s="8">
@@ -4110,7 +5292,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>64</v>
       </c>
@@ -4194,28 +5376,28 @@
       <c r="AA25" s="11">
         <v>1.0775603291504301</v>
       </c>
-      <c r="AB25" s="11">
+      <c r="AB25" s="12">
         <v>0.226238153882035</v>
       </c>
-      <c r="AC25" s="11">
+      <c r="AC25" s="12">
         <v>0.22452820272329299</v>
       </c>
-      <c r="AD25" s="11">
+      <c r="AD25" s="12">
         <v>1.00448304943463</v>
       </c>
-      <c r="AE25" s="11">
+      <c r="AE25" s="12">
         <v>1.00887794275822</v>
       </c>
-      <c r="AF25" s="11">
+      <c r="AF25" s="12">
         <v>0.223931545042724</v>
       </c>
-      <c r="AG25" s="11">
+      <c r="AG25" s="12">
         <v>0.227427296786546</v>
       </c>
-      <c r="AH25" s="11">
+      <c r="AH25" s="12">
         <v>0.22457541624059399</v>
       </c>
-      <c r="AI25" s="11">
+      <c r="AI25" s="12">
         <v>0.228075243272061</v>
       </c>
       <c r="AK25" s="8">
@@ -4247,7 +5429,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>56</v>
       </c>
@@ -4276,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>57</v>
       </c>
@@ -4305,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>58</v>
       </c>
@@ -4334,11 +5516,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:45" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="D29" s="22"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
+      <c r="AE29" s="12"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+      <c r="AH29" s="12"/>
+      <c r="AI29" s="12"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>59</v>
       </c>
@@ -4422,28 +5612,28 @@
       <c r="AA30" s="11">
         <v>2.02261078353864</v>
       </c>
-      <c r="AB30" s="11">
+      <c r="AB30" s="12">
         <v>0.27563114192600702</v>
       </c>
-      <c r="AC30" s="11">
+      <c r="AC30" s="12">
         <v>0.25904437352542797</v>
       </c>
-      <c r="AD30" s="11">
+      <c r="AD30" s="12">
         <v>0.36859362327181699</v>
       </c>
-      <c r="AE30" s="11">
+      <c r="AE30" s="12">
         <v>701988.13226680795</v>
       </c>
-      <c r="AF30" s="11">
+      <c r="AF30" s="12">
         <v>0.224128297096989</v>
       </c>
-      <c r="AG30" s="11">
+      <c r="AG30" s="12">
         <v>0.171398208347292</v>
       </c>
-      <c r="AH30" s="11">
+      <c r="AH30" s="12">
         <v>0.220464806283273</v>
       </c>
-      <c r="AI30" s="11">
+      <c r="AI30" s="12">
         <v>0.169685179990819</v>
       </c>
       <c r="AK30" s="8">
@@ -4475,7 +5665,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>60</v>
       </c>
@@ -4559,28 +5749,28 @@
       <c r="AA31" s="11">
         <v>1.54440724010301</v>
       </c>
-      <c r="AB31" s="11">
+      <c r="AB31" s="12">
         <v>0.24626361351909301</v>
       </c>
-      <c r="AC31" s="11">
+      <c r="AC31" s="12">
         <v>0.24120819475380301</v>
       </c>
-      <c r="AD31" s="11">
+      <c r="AD31" s="12">
         <v>0.68869880606447298</v>
       </c>
-      <c r="AE31" s="11">
+      <c r="AE31" s="12">
         <v>677245.82283571502</v>
       </c>
-      <c r="AF31" s="11">
+      <c r="AF31" s="12">
         <v>0.19846238033923599</v>
       </c>
-      <c r="AG31" s="11">
+      <c r="AG31" s="12">
         <v>0.21071716380093999</v>
       </c>
-      <c r="AH31" s="11">
+      <c r="AH31" s="12">
         <v>0.19681924210662799</v>
       </c>
-      <c r="AI31" s="11">
+      <c r="AI31" s="12">
         <v>0.20903642738095701</v>
       </c>
       <c r="AK31" s="8">
@@ -4612,7 +5802,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>61</v>
       </c>
@@ -4696,28 +5886,28 @@
       <c r="AA32" s="11">
         <v>1.1447400470706299</v>
       </c>
-      <c r="AB32" s="11">
+      <c r="AB32" s="12">
         <v>0.21620778467387899</v>
       </c>
-      <c r="AC32" s="11">
+      <c r="AC32" s="12">
         <v>0.21862724502845601</v>
       </c>
-      <c r="AD32" s="11">
+      <c r="AD32" s="12">
         <v>0.841212694220833</v>
       </c>
-      <c r="AE32" s="11">
+      <c r="AE32" s="12">
         <v>844945.51650394604</v>
       </c>
-      <c r="AF32" s="11">
+      <c r="AF32" s="12">
         <v>0.244781848979301</v>
       </c>
-      <c r="AG32" s="11">
+      <c r="AG32" s="12">
         <v>0.239414926760039</v>
       </c>
-      <c r="AH32" s="11">
+      <c r="AH32" s="12">
         <v>0.24416994254726801</v>
       </c>
-      <c r="AI32" s="11">
+      <c r="AI32" s="12">
         <v>0.23885082786207701</v>
       </c>
       <c r="AK32" s="8">
@@ -4749,7 +5939,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>62</v>
       </c>
@@ -4833,28 +6023,28 @@
       <c r="AA33" s="11">
         <v>1.9168051352767499</v>
       </c>
-      <c r="AB33" s="11">
+      <c r="AB33" s="12">
         <v>0.28030820868696898</v>
       </c>
-      <c r="AC33" s="11">
+      <c r="AC33" s="12">
         <v>0.27205757247484702</v>
       </c>
-      <c r="AD33" s="11">
+      <c r="AD33" s="12">
         <v>0.72820049213712701</v>
       </c>
-      <c r="AE33" s="11">
+      <c r="AE33" s="12">
         <v>713011.33081201301</v>
       </c>
-      <c r="AF33" s="11">
+      <c r="AF33" s="12">
         <v>0.129882799657212</v>
       </c>
-      <c r="AG33" s="11">
+      <c r="AG33" s="12">
         <v>0.146257841553633</v>
       </c>
-      <c r="AH33" s="11">
+      <c r="AH33" s="12">
         <v>0.12782111221725601</v>
       </c>
-      <c r="AI33" s="11">
+      <c r="AI33" s="12">
         <v>0.14433581882982199</v>
       </c>
       <c r="AK33" s="8">
@@ -4886,7 +6076,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>63</v>
       </c>
@@ -4970,28 +6160,28 @@
       <c r="AA34" s="11">
         <v>1.4890735624161899</v>
       </c>
-      <c r="AB34" s="11">
+      <c r="AB34" s="12">
         <v>0.241124635428108</v>
       </c>
-      <c r="AC34" s="11">
+      <c r="AC34" s="12">
         <v>0.23699932852450201</v>
       </c>
-      <c r="AD34" s="11">
+      <c r="AD34" s="12">
         <v>0.69346394054277205</v>
       </c>
-      <c r="AE34" s="11">
+      <c r="AE34" s="12">
         <v>688290.22268540005</v>
       </c>
-      <c r="AF34" s="11">
+      <c r="AF34" s="12">
         <v>0.20853605639149</v>
       </c>
-      <c r="AG34" s="11">
+      <c r="AG34" s="12">
         <v>0.21806638440788301</v>
       </c>
-      <c r="AH34" s="11">
+      <c r="AH34" s="12">
         <v>0.206962761175672</v>
       </c>
-      <c r="AI34" s="11">
+      <c r="AI34" s="12">
         <v>0.216478889235766</v>
       </c>
       <c r="AK34" s="8">
@@ -5011,7 +6201,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>64</v>
       </c>
@@ -5095,28 +6285,28 @@
       <c r="AA35" s="11">
         <v>1.1329531812066</v>
       </c>
-      <c r="AB35" s="11">
+      <c r="AB35" s="12">
         <v>0.22160109823218599</v>
       </c>
-      <c r="AC35" s="11">
+      <c r="AC35" s="12">
         <v>0.22459853490915499</v>
       </c>
-      <c r="AD35" s="11">
+      <c r="AD35" s="12">
         <v>0.83971515777780004</v>
       </c>
-      <c r="AE35" s="11">
+      <c r="AE35" s="12">
         <v>838176.45183920197</v>
       </c>
-      <c r="AF35" s="11">
+      <c r="AF35" s="12">
         <v>0.23373001354784501</v>
       </c>
-      <c r="AG35" s="11">
+      <c r="AG35" s="12">
         <v>0.22757172306228601</v>
       </c>
-      <c r="AH35" s="11">
+      <c r="AH35" s="12">
         <v>0.23315257931750399</v>
       </c>
-      <c r="AI35" s="11">
+      <c r="AI35" s="12">
         <v>0.227006506769517</v>
       </c>
       <c r="AK35" s="8">
@@ -5148,7 +6338,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>56</v>
       </c>
@@ -5177,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>57</v>
       </c>
@@ -5206,7 +6396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>58</v>
       </c>
@@ -5249,24 +6439,1945 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J20" sqref="J20"/>
+    </sheetView>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="23.44140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="23" customWidth="1"/>
+    <col min="7" max="9" width="9.21875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.21875" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" style="21" customWidth="1"/>
+    <col min="14" max="15" width="9.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="9.21875" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="9.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="9.109375" style="8"/>
+    <col min="28" max="31" width="9.109375" style="9"/>
+    <col min="32" max="32" width="9.109375" style="12"/>
+    <col min="33" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="20">
+        <v>1.0625752451781001</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="23">
+        <v>75.641399153779901</v>
+      </c>
+      <c r="G2" s="23">
+        <v>64.934223048097095</v>
+      </c>
+      <c r="H2" s="23">
+        <v>75.386214019546799</v>
+      </c>
+      <c r="I2" s="23">
+        <v>64.9947692291408</v>
+      </c>
+      <c r="J2" s="27">
+        <v>1.0000348015760001</v>
+      </c>
+      <c r="K2" s="27">
+        <v>1.0000348015181</v>
+      </c>
+      <c r="L2" s="21">
+        <v>-47.594386411072399</v>
+      </c>
+      <c r="M2" s="21">
+        <v>-47.594393635716798</v>
+      </c>
+      <c r="N2" s="21">
+        <v>-4.7652271006345603E-5</v>
+      </c>
+      <c r="O2" s="21">
+        <v>2.70456250689789E-5</v>
+      </c>
+      <c r="P2" s="33">
+        <v>35.813185534648198</v>
+      </c>
+      <c r="Q2" s="33">
+        <v>34.240381451573697</v>
+      </c>
+      <c r="R2" s="33">
+        <v>42.033617349066397</v>
+      </c>
+      <c r="S2" s="33">
+        <v>40.213791670643303</v>
+      </c>
+      <c r="T2" s="21">
+        <v>1.16585518705835</v>
+      </c>
+      <c r="U2" s="21">
+        <v>1.10390590779383</v>
+      </c>
+      <c r="V2" s="21">
+        <v>1.3434397395942399</v>
+      </c>
+      <c r="W2" s="21">
+        <v>1.29031211126889</v>
+      </c>
+      <c r="AF2" s="12">
+        <f>MIN(X2:AE2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="20">
+        <v>1.3351907809458401</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="23">
+        <v>76.672195353560298</v>
+      </c>
+      <c r="G3" s="23">
+        <v>64.731332031464106</v>
+      </c>
+      <c r="H3" s="23">
+        <v>76.516483868026697</v>
+      </c>
+      <c r="I3" s="23">
+        <v>64.807228534427395</v>
+      </c>
+      <c r="J3" s="27">
+        <v>1.00003480155008</v>
+      </c>
+      <c r="K3" s="27">
+        <v>1.0000348018690599</v>
+      </c>
+      <c r="L3" s="21">
+        <v>-47.594389645088803</v>
+      </c>
+      <c r="M3" s="21">
+        <v>-47.5943498398576</v>
+      </c>
+      <c r="N3" s="21">
+        <v>5.8149457273096401E-6</v>
+      </c>
+      <c r="O3" s="21">
+        <v>6.2784830065057797E-4</v>
+      </c>
+      <c r="P3" s="33">
+        <v>31.408387118243098</v>
+      </c>
+      <c r="Q3" s="33">
+        <v>29.764640086972499</v>
+      </c>
+      <c r="R3" s="33">
+        <v>38.121990019530799</v>
+      </c>
+      <c r="S3" s="33">
+        <v>36.188669098408198</v>
+      </c>
+      <c r="T3" s="21">
+        <v>1.0261165882519701</v>
+      </c>
+      <c r="U3" s="21">
+        <v>0.96325862604463097</v>
+      </c>
+      <c r="V3" s="21">
+        <v>1.2206442259115899</v>
+      </c>
+      <c r="W3" s="21">
+        <v>1.16435727283803</v>
+      </c>
+      <c r="AF3" s="12">
+        <f t="shared" ref="AF3:AF38" si="0">MIN(X3:AE3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="20">
+        <v>1.56728058309068</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="23">
+        <v>65.428841883969298</v>
+      </c>
+      <c r="G4" s="23">
+        <v>76.134888072171506</v>
+      </c>
+      <c r="H4" s="23">
+        <v>75.840853769650295</v>
+      </c>
+      <c r="I4" s="23">
+        <v>65.380555460854396</v>
+      </c>
+      <c r="J4" s="27">
+        <v>1.00003480153895</v>
+      </c>
+      <c r="K4" s="27">
+        <v>1.0000348015206899</v>
+      </c>
+      <c r="L4" s="21">
+        <v>-47.594391034473603</v>
+      </c>
+      <c r="M4" s="21">
+        <v>-47.594393312798402</v>
+      </c>
+      <c r="N4" s="21">
+        <v>1.7759518565465301E-6</v>
+      </c>
+      <c r="O4" s="21">
+        <v>4.66340450169149E-5</v>
+      </c>
+      <c r="P4" s="33">
+        <v>36.382772671423098</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>32.924967511917302</v>
+      </c>
+      <c r="R4" s="33">
+        <v>29.483103927726798</v>
+      </c>
+      <c r="S4" s="33">
+        <v>39.383145618287102</v>
+      </c>
+      <c r="T4" s="21">
+        <v>1.1826526981068799</v>
+      </c>
+      <c r="U4" s="21">
+        <v>1.0645420592016199</v>
+      </c>
+      <c r="V4" s="21">
+        <v>0.94457560944360797</v>
+      </c>
+      <c r="W4" s="21">
+        <v>1.2741566849569299</v>
+      </c>
+      <c r="AF4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1.81219298226804</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="23">
+        <v>77.361906300916402</v>
+      </c>
+      <c r="G5" s="23">
+        <v>65.314816818828902</v>
+      </c>
+      <c r="H5" s="23">
+        <v>65.492499586053</v>
+      </c>
+      <c r="I5" s="23">
+        <v>76.214936993037597</v>
+      </c>
+      <c r="J5" s="27">
+        <v>1.0000347929025399</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1.0000347995477601</v>
+      </c>
+      <c r="L5" s="21">
+        <v>-47.595468901778702</v>
+      </c>
+      <c r="M5" s="21">
+        <v>-47.594639520767998</v>
+      </c>
+      <c r="N5" s="21">
+        <v>-6.3600467912478095E-4</v>
+      </c>
+      <c r="O5" s="21">
+        <v>-2.15729623685688E-3</v>
+      </c>
+      <c r="P5" s="33">
+        <v>29.662311562906901</v>
+      </c>
+      <c r="Q5" s="33">
+        <v>35.927092214352399</v>
+      </c>
+      <c r="R5" s="33">
+        <v>37.865174150855204</v>
+      </c>
+      <c r="S5" s="33">
+        <v>28.983947285811801</v>
+      </c>
+      <c r="T5" s="21">
+        <v>0.97135899803911196</v>
+      </c>
+      <c r="U5" s="21">
+        <v>1.1700413341404601</v>
+      </c>
+      <c r="V5" s="21">
+        <v>1.2238644545366399</v>
+      </c>
+      <c r="W5" s="21">
+        <v>0.92769022158547199</v>
+      </c>
+      <c r="AF5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="20">
+        <v>2.0529370827241</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="23">
+        <v>65.801661804920201</v>
+      </c>
+      <c r="G6" s="23">
+        <v>77.110428743580798</v>
+      </c>
+      <c r="H6" s="23">
+        <v>76.6054083100219</v>
+      </c>
+      <c r="I6" s="23">
+        <v>65.642950459765899</v>
+      </c>
+      <c r="J6" s="27">
+        <v>1.00003480167558</v>
+      </c>
+      <c r="K6" s="27">
+        <v>1.00003480688532</v>
+      </c>
+      <c r="L6" s="21">
+        <v>-47.594373983873503</v>
+      </c>
+      <c r="M6" s="21">
+        <v>-47.593723913637703</v>
+      </c>
+      <c r="N6" s="21">
+        <v>9.7817343298834802E-4</v>
+      </c>
+      <c r="O6" s="21">
+        <v>6.1054152838853999E-3</v>
+      </c>
+      <c r="P6" s="33">
+        <v>34.136995460881302</v>
+      </c>
+      <c r="Q6" s="33">
+        <v>29.6607708044573</v>
+      </c>
+      <c r="R6" s="33">
+        <v>26.781773039116501</v>
+      </c>
+      <c r="S6" s="33">
+        <v>36.701716683025602</v>
+      </c>
+      <c r="T6" s="21">
+        <v>1.1212418709902401</v>
+      </c>
+      <c r="U6" s="21">
+        <v>0.958924118713817</v>
+      </c>
+      <c r="V6" s="21">
+        <v>0.86099889594613499</v>
+      </c>
+      <c r="W6" s="21">
+        <v>1.19762861920816</v>
+      </c>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="AF6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="20">
+        <v>2.4462693228308301</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="23">
+        <v>66.034651350854105</v>
+      </c>
+      <c r="G7" s="23">
+        <v>78.019410363957206</v>
+      </c>
+      <c r="H7" s="23">
+        <v>77.241347511665296</v>
+      </c>
+      <c r="I7" s="23">
+        <v>65.762927788006607</v>
+      </c>
+      <c r="J7" s="27">
+        <v>1.0000347896016</v>
+      </c>
+      <c r="K7" s="27">
+        <v>1.00003479886034</v>
+      </c>
+      <c r="L7" s="21">
+        <v>-47.595880946786501</v>
+      </c>
+      <c r="M7" s="21">
+        <v>-47.594725309989201</v>
+      </c>
+      <c r="N7" s="21">
+        <v>-1.33219642311997E-2</v>
+      </c>
+      <c r="O7" s="21">
+        <v>-3.4351995678164899E-3</v>
+      </c>
+      <c r="P7" s="33">
+        <v>32.535083237329303</v>
+      </c>
+      <c r="Q7" s="33">
+        <v>26.902766825842601</v>
+      </c>
+      <c r="R7" s="33">
+        <v>24.398019437840102</v>
+      </c>
+      <c r="S7" s="33">
+        <v>34.590057357682902</v>
+      </c>
+      <c r="T7" s="21">
+        <v>1.0745872560959699</v>
+      </c>
+      <c r="U7" s="21">
+        <v>0.86700511757217202</v>
+      </c>
+      <c r="V7" s="21">
+        <v>0.78471759517059403</v>
+      </c>
+      <c r="W7" s="21">
+        <v>1.13385388003528</v>
+      </c>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="AF7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D8" s="20">
+        <v>2.6533946851368002</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="23">
+        <v>66.302616186005807</v>
+      </c>
+      <c r="G8" s="23">
+        <v>78.085800133114404</v>
+      </c>
+      <c r="H8" s="23">
+        <v>77.396275596628897</v>
+      </c>
+      <c r="I8" s="23">
+        <v>65.936290586986303</v>
+      </c>
+      <c r="J8" s="27">
+        <v>1.0000348015396101</v>
+      </c>
+      <c r="K8" s="27">
+        <v>1.00003480271956</v>
+      </c>
+      <c r="L8" s="21">
+        <v>-47.594390951843003</v>
+      </c>
+      <c r="M8" s="21">
+        <v>-47.5942437090402</v>
+      </c>
+      <c r="N8" s="21">
+        <v>-3.9858019298584502E-4</v>
+      </c>
+      <c r="O8" s="21">
+        <v>1.0361249789656399E-3</v>
+      </c>
+      <c r="P8" s="33">
+        <v>31.8825731509056</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>26.177498761943198</v>
+      </c>
+      <c r="R8" s="33">
+        <v>24.060672965327299</v>
+      </c>
+      <c r="S8" s="33">
+        <v>33.383383605859898</v>
+      </c>
+      <c r="T8" s="21">
+        <v>1.0603673743791</v>
+      </c>
+      <c r="U8" s="21">
+        <v>0.84319488535345499</v>
+      </c>
+      <c r="V8" s="21">
+        <v>0.77326033255209403</v>
+      </c>
+      <c r="W8" s="21">
+        <v>1.1013538463852</v>
+      </c>
+      <c r="AF8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D9" s="20">
+        <v>2.90565590947116</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="23">
+        <v>65.441717784998701</v>
+      </c>
+      <c r="G9" s="33">
+        <v>83.889321770245104</v>
+      </c>
+      <c r="H9" s="23">
+        <v>65.504540029421406</v>
+      </c>
+      <c r="I9" s="23">
+        <v>85.228075867455303</v>
+      </c>
+      <c r="J9" s="27">
+        <v>1.0000348010834801</v>
+      </c>
+      <c r="K9" s="27">
+        <v>1.0000348017109799</v>
+      </c>
+      <c r="L9" s="21">
+        <v>-47.5944478716455</v>
+      </c>
+      <c r="M9" s="21">
+        <v>-47.594369566120399</v>
+      </c>
+      <c r="N9" s="21">
+        <v>-4.5510636409883901E-4</v>
+      </c>
+      <c r="O9" s="21">
+        <v>-3.3917126360186001E-3</v>
+      </c>
+      <c r="P9" s="33">
+        <v>26.4547344308288</v>
+      </c>
+      <c r="Q9" s="33">
+        <v>25.879313877420898</v>
+      </c>
+      <c r="R9" s="33">
+        <v>15.674505084585601</v>
+      </c>
+      <c r="S9" s="33">
+        <v>14.9908840142812</v>
+      </c>
+      <c r="T9" s="21">
+        <v>0.86491585875233101</v>
+      </c>
+      <c r="U9" s="21">
+        <v>0.84768438692215697</v>
+      </c>
+      <c r="V9" s="21">
+        <v>0.50821917360503799</v>
+      </c>
+      <c r="W9" s="21">
+        <v>0.49171676519700003</v>
+      </c>
+      <c r="AF9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="D10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="12"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1.0625752451781001</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="23">
+        <v>63.750590174852398</v>
+      </c>
+      <c r="G11" s="23">
+        <v>75.971792605489298</v>
+      </c>
+      <c r="H11" s="23">
+        <v>63.275559294582898</v>
+      </c>
+      <c r="I11" s="23">
+        <v>76.344923473460597</v>
+      </c>
+      <c r="J11" s="27">
+        <v>1.6473716018615601</v>
+      </c>
+      <c r="K11" s="27">
+        <v>1.64737157399684</v>
+      </c>
+      <c r="L11" s="21">
+        <v>-6.1166126154366696</v>
+      </c>
+      <c r="M11" s="21">
+        <v>-6.1166127566580304</v>
+      </c>
+      <c r="N11" s="21">
+        <v>-75.841769176503803</v>
+      </c>
+      <c r="O11" s="21">
+        <v>-75.841766859126594</v>
+      </c>
+      <c r="P11" s="33">
+        <v>35.052224605415802</v>
+      </c>
+      <c r="Q11" s="33">
+        <v>34.271621364304103</v>
+      </c>
+      <c r="R11" s="33">
+        <v>35.6954771578907</v>
+      </c>
+      <c r="S11" s="33">
+        <v>34.763645900052097</v>
+      </c>
+      <c r="T11" s="21">
+        <v>1.1300045597716399</v>
+      </c>
+      <c r="U11" s="21">
+        <v>1.0969304951340599</v>
+      </c>
+      <c r="V11" s="21">
+        <v>1.1407746297951</v>
+      </c>
+      <c r="W11" s="21">
+        <v>1.1150037704168301</v>
+      </c>
+      <c r="AF11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1.3351907809458401</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="23">
+        <v>63.302561142202798</v>
+      </c>
+      <c r="G12" s="23">
+        <v>76.901163008109094</v>
+      </c>
+      <c r="H12" s="23">
+        <v>62.810652558296802</v>
+      </c>
+      <c r="I12" s="23">
+        <v>77.429834019339097</v>
+      </c>
+      <c r="J12" s="27">
+        <v>1.6473715945090901</v>
+      </c>
+      <c r="K12" s="27">
+        <v>1.64737159378668</v>
+      </c>
+      <c r="L12" s="21">
+        <v>-6.1166126526997697</v>
+      </c>
+      <c r="M12" s="21">
+        <v>-6.1166126563610197</v>
+      </c>
+      <c r="N12" s="21">
+        <v>-75.841767763183498</v>
+      </c>
+      <c r="O12" s="21">
+        <v>-75.841767526795095</v>
+      </c>
+      <c r="P12" s="33">
+        <v>31.320304968528301</v>
+      </c>
+      <c r="Q12" s="33">
+        <v>30.322375456767301</v>
+      </c>
+      <c r="R12" s="33">
+        <v>32.019949982898702</v>
+      </c>
+      <c r="S12" s="33">
+        <v>30.8782860676931</v>
+      </c>
+      <c r="T12" s="21">
+        <v>1.01171236344093</v>
+      </c>
+      <c r="U12" s="21">
+        <v>0.97319084086738905</v>
+      </c>
+      <c r="V12" s="21">
+        <v>1.02527736441294</v>
+      </c>
+      <c r="W12" s="21">
+        <v>0.99322852461408495</v>
+      </c>
+      <c r="AF12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1.56728058309068</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="23">
+        <v>77.995447266131805</v>
+      </c>
+      <c r="G13" s="23">
+        <v>62.661893713801703</v>
+      </c>
+      <c r="H13" s="23">
+        <v>77.884535456353305</v>
+      </c>
+      <c r="I13" s="23">
+        <v>62.600758071921398</v>
+      </c>
+      <c r="J13" s="27">
+        <v>1.64737159442008</v>
+      </c>
+      <c r="K13" s="27">
+        <v>1.6473715939245299</v>
+      </c>
+      <c r="L13" s="21">
+        <v>-6.1166126531509102</v>
+      </c>
+      <c r="M13" s="21">
+        <v>-6.1166126556623803</v>
+      </c>
+      <c r="N13" s="21">
+        <v>-75.841767822853299</v>
+      </c>
+      <c r="O13" s="21">
+        <v>-75.8417676979644</v>
+      </c>
+      <c r="P13" s="33">
+        <v>31.405780251239602</v>
+      </c>
+      <c r="Q13" s="33">
+        <v>30.089978717979999</v>
+      </c>
+      <c r="R13" s="33">
+        <v>30.4228790713771</v>
+      </c>
+      <c r="S13" s="33">
+        <v>28.590931612802201</v>
+      </c>
+      <c r="T13" s="21">
+        <v>1.0249324169434999</v>
+      </c>
+      <c r="U13" s="21">
+        <v>0.97424994544815202</v>
+      </c>
+      <c r="V13" s="21">
+        <v>0.97552970065852596</v>
+      </c>
+      <c r="W13" s="21">
+        <v>0.92210075879276399</v>
+      </c>
+      <c r="AF13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="20">
+        <v>1.81219298226804</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="23">
+        <v>77.731571113105602</v>
+      </c>
+      <c r="G14" s="23">
+        <v>63.561483212179397</v>
+      </c>
+      <c r="H14" s="23">
+        <v>63.791945757673801</v>
+      </c>
+      <c r="I14" s="23">
+        <v>76.826919766356497</v>
+      </c>
+      <c r="J14" s="27">
+        <v>1.64737159629049</v>
+      </c>
+      <c r="K14" s="27">
+        <v>1.64737160001537</v>
+      </c>
+      <c r="L14" s="21">
+        <v>-6.1166126436714396</v>
+      </c>
+      <c r="M14" s="21">
+        <v>-6.1166126247933699</v>
+      </c>
+      <c r="N14" s="21">
+        <v>-75.841767705145699</v>
+      </c>
+      <c r="O14" s="21">
+        <v>-75.841769315405401</v>
+      </c>
+      <c r="P14" s="33">
+        <v>33.318103814396999</v>
+      </c>
+      <c r="Q14" s="33">
+        <v>31.4141454422018</v>
+      </c>
+      <c r="R14" s="33">
+        <v>32.867796017930303</v>
+      </c>
+      <c r="S14" s="33">
+        <v>32.849974681021997</v>
+      </c>
+      <c r="T14" s="21">
+        <v>1.0896030593813799</v>
+      </c>
+      <c r="U14" s="21">
+        <v>1.0261643911484699</v>
+      </c>
+      <c r="V14" s="21">
+        <v>1.06340780767079</v>
+      </c>
+      <c r="W14" s="21">
+        <v>1.05528369701574</v>
+      </c>
+      <c r="AF14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D15" s="20">
+        <v>2.0529370827241</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="23">
+        <v>78.224191797845407</v>
+      </c>
+      <c r="G15" s="23">
+        <v>63.640528381194201</v>
+      </c>
+      <c r="H15" s="23">
+        <v>63.763837431969598</v>
+      </c>
+      <c r="I15" s="23">
+        <v>77.107663858949707</v>
+      </c>
+      <c r="J15" s="27">
+        <v>1.6473715885139</v>
+      </c>
+      <c r="K15" s="27">
+        <v>1.6473715956862101</v>
+      </c>
+      <c r="L15" s="21">
+        <v>-6.1166126830840097</v>
+      </c>
+      <c r="M15" s="21">
+        <v>-6.1166126467340103</v>
+      </c>
+      <c r="N15" s="21">
+        <v>-75.841767229539698</v>
+      </c>
+      <c r="O15" s="21">
+        <v>-75.841767569494095</v>
+      </c>
+      <c r="P15" s="33">
+        <v>31.9426397389099</v>
+      </c>
+      <c r="Q15" s="33">
+        <v>30.061101909044801</v>
+      </c>
+      <c r="R15" s="33">
+        <v>31.689765129941001</v>
+      </c>
+      <c r="S15" s="33">
+        <v>31.771874025007101</v>
+      </c>
+      <c r="T15" s="21">
+        <v>1.0469514477127999</v>
+      </c>
+      <c r="U15" s="21">
+        <v>0.98644811252825404</v>
+      </c>
+      <c r="V15" s="21">
+        <v>1.0300436911462501</v>
+      </c>
+      <c r="W15" s="21">
+        <v>1.02137320768518</v>
+      </c>
+      <c r="AF15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="20">
+        <v>2.4462693228308301</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="23">
+        <v>63.9961414697161</v>
+      </c>
+      <c r="G16" s="23">
+        <v>78.167410124486807</v>
+      </c>
+      <c r="H16" s="23">
+        <v>77.554607723937806</v>
+      </c>
+      <c r="I16" s="23">
+        <v>63.695791366860398</v>
+      </c>
+      <c r="J16" s="27">
+        <v>1.64737158247934</v>
+      </c>
+      <c r="K16" s="27">
+        <v>1.64737159324572</v>
+      </c>
+      <c r="L16" s="21">
+        <v>-6.1166127136678101</v>
+      </c>
+      <c r="M16" s="21">
+        <v>-6.1166126591026799</v>
+      </c>
+      <c r="N16" s="21">
+        <v>-75.841766414467301</v>
+      </c>
+      <c r="O16" s="21">
+        <v>-75.841767528141901</v>
+      </c>
+      <c r="P16" s="33">
+        <v>27.457981790726802</v>
+      </c>
+      <c r="Q16" s="33">
+        <v>31.399787926859599</v>
+      </c>
+      <c r="R16" s="33">
+        <v>28.934847358216</v>
+      </c>
+      <c r="S16" s="33">
+        <v>29.754653430805099</v>
+      </c>
+      <c r="T16" s="21">
+        <v>0.91308888262914301</v>
+      </c>
+      <c r="U16" s="21">
+        <v>1.01598806499522</v>
+      </c>
+      <c r="V16" s="21">
+        <v>0.93371862094676195</v>
+      </c>
+      <c r="W16" s="21">
+        <v>0.97654393517861504</v>
+      </c>
+      <c r="AF16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2.6533946851368002</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="23">
+        <v>64.190642495275</v>
+      </c>
+      <c r="G17" s="23">
+        <v>78.245674953220103</v>
+      </c>
+      <c r="H17" s="23">
+        <v>77.756451423679295</v>
+      </c>
+      <c r="I17" s="23">
+        <v>63.7570469670191</v>
+      </c>
+      <c r="J17" s="27">
+        <v>1.6473715944229901</v>
+      </c>
+      <c r="K17" s="27">
+        <v>1.6473715948780501</v>
+      </c>
+      <c r="L17" s="21">
+        <v>-6.11661265313613</v>
+      </c>
+      <c r="M17" s="21">
+        <v>-6.1166126508298602</v>
+      </c>
+      <c r="N17" s="21">
+        <v>-75.841767724800405</v>
+      </c>
+      <c r="O17" s="21">
+        <v>-75.841767776815004</v>
+      </c>
+      <c r="P17" s="33">
+        <v>26.907794747513702</v>
+      </c>
+      <c r="Q17" s="33">
+        <v>30.771136164828</v>
+      </c>
+      <c r="R17" s="33">
+        <v>28.7841102946022</v>
+      </c>
+      <c r="S17" s="33">
+        <v>28.7157250148428</v>
+      </c>
+      <c r="T17" s="21">
+        <v>0.90122862622775102</v>
+      </c>
+      <c r="U17" s="21">
+        <v>0.99702216844223601</v>
+      </c>
+      <c r="V17" s="21">
+        <v>0.92998479473686702</v>
+      </c>
+      <c r="W17" s="21">
+        <v>0.94813262674758403</v>
+      </c>
+      <c r="AF17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="20">
+        <v>2.90565590947116</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="23">
+        <v>64.219262162626293</v>
+      </c>
+      <c r="G18" s="23">
+        <v>78.398500591817296</v>
+      </c>
+      <c r="H18" s="23">
+        <v>77.996827142251803</v>
+      </c>
+      <c r="I18" s="23">
+        <v>63.838181087531503</v>
+      </c>
+      <c r="J18" s="27">
+        <v>1.6473715945099401</v>
+      </c>
+      <c r="K18" s="27">
+        <v>1.6473715945026</v>
+      </c>
+      <c r="L18" s="21">
+        <v>-6.1166126526954798</v>
+      </c>
+      <c r="M18" s="21">
+        <v>-6.1166126527326599</v>
+      </c>
+      <c r="N18" s="21">
+        <v>-75.841767721885603</v>
+      </c>
+      <c r="O18" s="21">
+        <v>-75.841767719631605</v>
+      </c>
+      <c r="P18" s="33">
+        <v>25.849468302041899</v>
+      </c>
+      <c r="Q18" s="33">
+        <v>30.098664772862001</v>
+      </c>
+      <c r="R18" s="33">
+        <v>28.317235435339899</v>
+      </c>
+      <c r="S18" s="33">
+        <v>27.6610731303617</v>
+      </c>
+      <c r="T18" s="21">
+        <v>0.871766295879709</v>
+      </c>
+      <c r="U18" s="21">
+        <v>0.97693949628643795</v>
+      </c>
+      <c r="V18" s="21">
+        <v>0.91628488557881704</v>
+      </c>
+      <c r="W18" s="21">
+        <v>0.91946866510759395</v>
+      </c>
+      <c r="AF18" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="D19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.394233691326</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF20" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.80477500408199998</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="20">
+        <v>1.7076141356200001</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.42156602891900002</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF23" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.87657298072099998</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF24" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="1">
+        <v>55</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="20">
+        <v>1.81570768537</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF25" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A26" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="1">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.44813940335699998</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF26" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="20">
+        <v>0.93957194533599997</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF27" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D28" s="20">
+        <v>1.89434550845</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF28" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="D29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0.394233691326</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X30" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="Y30" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="Z30" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="AA30" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="AB30" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="AC30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE30" s="9">
+        <v>1.25</v>
+      </c>
+      <c r="AF30" s="12">
+        <f t="shared" si="0"/>
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.80477500408199998</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X31" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="Y31" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Z31" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="AA31" s="8">
+        <v>1.23</v>
+      </c>
+      <c r="AB31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF31" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1">
+        <v>55</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="20">
+        <v>1.7076141356200001</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="Y32" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="Z32" s="8">
+        <v>1.48</v>
+      </c>
+      <c r="AA32" s="8">
+        <v>1.58</v>
+      </c>
+      <c r="AB32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF32" s="12">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="1">
+        <v>55</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="20">
+        <v>0.42156602891900002</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X33" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="Y33" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="Z33" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="AA33" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AB33" s="9">
+        <v>1.44</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE33" s="9">
+        <v>1.39</v>
+      </c>
+      <c r="AF33" s="12">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1">
+        <v>55</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D34" s="20">
+        <v>0.87657298072099998</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X34" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Y34" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="Z34" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA34" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="AF34" s="12">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1">
+        <v>55</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D35" s="20">
+        <v>1.81570768537</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X35" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="Y35" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="Z35" s="8">
+        <v>1.74</v>
+      </c>
+      <c r="AA35" s="8">
+        <v>1.83</v>
+      </c>
+      <c r="AB35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF35" s="12">
+        <f t="shared" si="0"/>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1">
+        <v>55</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D36" s="20">
+        <v>0.44813940335699998</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" s="27">
+        <f t="shared" ref="J36:K38" si="1">(1+L36)/(1-L36)</f>
+        <v>1</v>
+      </c>
+      <c r="K36" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A37" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="1">
+        <v>55</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D37" s="20">
+        <v>0.93957194533599997</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A38" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="1">
+        <v>55</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D38" s="20">
+        <v>1.89434550845</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K38" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AF38" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>